<commit_message>
Optimized the shit out of the the telemetry module
</commit_message>
<xml_diff>
--- a/mod-data.xlsx
+++ b/mod-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Forge Projects\Mine Mine no Mi - 1.7.10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1DFB37-BAAD-4791-928F-0D25EE7D49AA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAE0058-2DF6-4EB9-A59A-0B5BA4CE9E60}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t>HP</t>
   </si>
@@ -87,24 +87,6 @@
     <t>Lapahn Jump</t>
   </si>
   <si>
-    <t>Individual POST</t>
-  </si>
-  <si>
-    <t>#</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Misc</t>
-  </si>
-  <si>
-    <t>Array POST</t>
-  </si>
-  <si>
-    <t>Size (in Bytes)</t>
-  </si>
-  <si>
     <t>Individual:</t>
   </si>
   <si>
@@ -127,13 +109,22 @@
   </si>
   <si>
     <t>Elements</t>
+  </si>
+  <si>
+    <t>Compound</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Elements (Inserts)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,13 +149,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -215,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -232,55 +216,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -291,30 +238,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F4C4A093-7EB5-4982-A088-1AEAABF88312}" name="Table1" displayName="Table1" ref="B5:D17" totalsRowShown="0" headerRowDxfId="5" dataDxfId="6">
-  <autoFilter ref="B5:D17" xr:uid="{3F3B0018-1131-4686-93C7-93C90C72F165}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{1B03EE42-96FD-47C6-B525-FC8FFABC3E29}" name="#" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{5EA1AADE-D6DF-4B9D-BB78-FA69FF77BA14}" name="Type" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{8B05CEEF-FBBF-4640-9D70-DEE9584AA513}" name="Size (in Bytes)" dataDxfId="7"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{75B93099-F6B6-44F6-90BF-47A91595F63F}" name="Table13" displayName="Table13" ref="G5:I17" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="G5:I17" xr:uid="{39E4AA52-7B22-4761-9063-75F335F7C713}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{2E1BC9F4-8E16-486F-BCA9-32918882D5C5}" name="#" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{278FE68B-4931-43AA-9219-1FCE7CDDC217}" name="Type" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{141D175B-431B-4F98-AFF8-05310ACE9360}" name="Size (in Bytes)" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -638,19 +561,19 @@
       <c r="M3" s="2"/>
     </row>
     <row r="4" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -739,21 +662,21 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
     </row>
     <row r="9" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -855,21 +778,21 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="7" t="s">
+      <c r="H13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
     <row r="14" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -1110,295 +1033,109 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8693409-BA59-48C5-9334-B63105C5D5CE}">
-  <dimension ref="B3:R17"/>
+  <dimension ref="B6:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
     <col min="8" max="8" width="11.85546875" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
     <col min="14" max="14" width="11.7109375" customWidth="1"/>
     <col min="17" max="17" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="2:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="B4" s="8" t="s">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="G4" s="8" t="s">
+      <c r="E6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+      <c r="H6" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="C8">
+        <v>88</v>
+      </c>
+      <c r="E8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="H8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <f>C7*C8</f>
+        <v>528</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9">
+        <v>534</v>
+      </c>
+      <c r="H9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="1">
-        <v>88</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="1">
-        <v>534</v>
-      </c>
-      <c r="N6" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q6" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="1">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="1">
-        <v>88</v>
-      </c>
-      <c r="G7" s="1">
-        <v>2</v>
-      </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="N7" t="s">
-        <v>24</v>
-      </c>
-      <c r="O7">
-        <f>COUNT(D6:D11)</f>
-        <v>6</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>24</v>
-      </c>
-      <c r="R7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="1">
-        <v>3</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="1">
-        <v>88</v>
-      </c>
-      <c r="G8" s="1">
-        <v>3</v>
-      </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="N8" t="s">
-        <v>25</v>
-      </c>
-      <c r="O8">
-        <f>AVERAGE(D6:D11)</f>
-        <v>88</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>30</v>
-      </c>
-      <c r="R8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="1">
-        <v>4</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="1">
-        <v>88</v>
-      </c>
-      <c r="G9" s="1">
-        <v>4</v>
-      </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="N9" t="s">
-        <v>26</v>
-      </c>
-      <c r="O9">
-        <f>O7*O8</f>
-        <v>528</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R9">
-        <f>I6</f>
-        <v>534</v>
-      </c>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="1">
-        <v>5</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="1">
-        <v>88</v>
-      </c>
-      <c r="G10" s="1">
-        <v>5</v>
-      </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="Q10" t="s">
-        <v>28</v>
-      </c>
-      <c r="R10">
-        <f>R9/R8</f>
+      <c r="F10">
+        <f>F9/F8</f>
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="1">
-        <v>6</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="1">
-        <v>88</v>
-      </c>
-      <c r="G11" s="1">
-        <v>6</v>
-      </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="1">
-        <v>7</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="G12" s="1">
-        <v>7</v>
-      </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="1">
-        <v>8</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="G13" s="1">
-        <v>8</v>
-      </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="1">
-        <v>9</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="G14" s="1">
-        <v>9</v>
-      </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="1">
-        <v>10</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="G15" s="1">
-        <v>10</v>
-      </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="1">
-        <v>11</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="G16" s="1">
-        <v>11</v>
-      </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="1">
-        <v>12</v>
-      </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="G17" s="1">
-        <v>12</v>
-      </c>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="G4:I4"/>
-  </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="2">
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the belly/doriki distribution based on the mod's threat level
</commit_message>
<xml_diff>
--- a/mod-data.xlsx
+++ b/mod-data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Forge Projects\Mine Mine no Mi - 1.7.10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAE0058-2DF6-4EB9-A59A-0B5BA4CE9E60}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FEFFE73-EC74-4A36-B0C5-92D067B7ACCC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="entity-balance" sheetId="1" r:id="rId1"/>
     <sheet name="http-size" sheetId="2" r:id="rId2"/>
+    <sheet name="drop distribution" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
   <si>
     <t>HP</t>
   </si>
@@ -118,6 +119,30 @@
   </si>
   <si>
     <t>Elements (Inserts)</t>
+  </si>
+  <si>
+    <t>Belly Distribution</t>
+  </si>
+  <si>
+    <t>Doriki Distribution</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>Avg:</t>
+  </si>
+  <si>
+    <t>Min:</t>
+  </si>
+  <si>
+    <t>Max:</t>
+  </si>
+  <si>
+    <t>Abs Min:</t>
+  </si>
+  <si>
+    <t>Abs Max:</t>
   </si>
 </sst>
 </file>
@@ -199,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -223,6 +248,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1035,7 +1064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8693409-BA59-48C5-9334-B63105C5D5CE}">
   <dimension ref="B6:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -1138,4 +1167,588 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6C50FA5-D05A-454C-81EF-B4135BD26674}">
+  <dimension ref="B3:J73"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>34</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="G3">
+        <v>52</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="9"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4">
+        <f>COUNTA(B:B)</f>
+        <v>71</v>
+      </c>
+      <c r="G4">
+        <v>65</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4">
+        <f>COUNTA(G:G)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>49</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="10">
+        <f>AVERAGE(B:B)</f>
+        <v>40.239436619718312</v>
+      </c>
+      <c r="G5">
+        <v>37</v>
+      </c>
+      <c r="I5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="10">
+        <f>AVERAGE(G:G)</f>
+        <v>58.674999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>47</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6">
+        <f>MIN(B:B)</f>
+        <v>21</v>
+      </c>
+      <c r="G6">
+        <v>53</v>
+      </c>
+      <c r="I6" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6">
+        <f>MIN(G:G)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="G7">
+        <v>59</v>
+      </c>
+      <c r="I7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>45</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8">
+        <f>MAX(B:B)</f>
+        <v>64</v>
+      </c>
+      <c r="G8">
+        <v>46</v>
+      </c>
+      <c r="I8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8">
+        <f>MAX(G:G)</f>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9">
+        <f>20+20+25</f>
+        <v>65</v>
+      </c>
+      <c r="G9">
+        <v>75</v>
+      </c>
+      <c r="I9" t="s">
+        <v>35</v>
+      </c>
+      <c r="J9">
+        <f>15+50+50</f>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>47</v>
+      </c>
+      <c r="G10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>36</v>
+      </c>
+      <c r="G11">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>35</v>
+      </c>
+      <c r="G12">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>52</v>
+      </c>
+      <c r="G13">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>34</v>
+      </c>
+      <c r="G14">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>32</v>
+      </c>
+      <c r="G15">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>44</v>
+      </c>
+      <c r="G16">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>34</v>
+      </c>
+      <c r="G17">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>26</v>
+      </c>
+      <c r="G18">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>40</v>
+      </c>
+      <c r="G19">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>43</v>
+      </c>
+      <c r="G20">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>43</v>
+      </c>
+      <c r="G21">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>54</v>
+      </c>
+      <c r="G22">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>42</v>
+      </c>
+      <c r="G23">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>38</v>
+      </c>
+      <c r="G24">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>41</v>
+      </c>
+      <c r="G25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>51</v>
+      </c>
+      <c r="G26">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>31</v>
+      </c>
+      <c r="G27">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>38</v>
+      </c>
+      <c r="G28">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>38</v>
+      </c>
+      <c r="G29">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>23</v>
+      </c>
+      <c r="G30">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>26</v>
+      </c>
+      <c r="G31">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>46</v>
+      </c>
+      <c r="G32">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>30</v>
+      </c>
+      <c r="G33">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>22</v>
+      </c>
+      <c r="G34">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>47</v>
+      </c>
+      <c r="G35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>41</v>
+      </c>
+      <c r="G36">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>38</v>
+      </c>
+      <c r="G37">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>48</v>
+      </c>
+      <c r="G38">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>31</v>
+      </c>
+      <c r="G39">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>34</v>
+      </c>
+      <c r="G40">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>21</v>
+      </c>
+      <c r="G41">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>35</v>
+      </c>
+      <c r="G42">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B60">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B61">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B62">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B64">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="I3:J3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>